<commit_message>
better read of sheets with missing data
</commit_message>
<xml_diff>
--- a/pyees/testData/data10.xlsx
+++ b/pyees/testData/data10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ymerdkdc01\folder redirections\DJAVE\My Documents\GitHub\pyees\pyees\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB22AC7-7471-43AC-A858-4FFE51333C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA12158-CF8E-45AC-9D6C-8A241EA7170B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F6BAB0-B9A3-4FB8-B84A-62DE77F5D537}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5F6BAB0-B9A3-4FB8-B84A-62DE77F5D537}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>A</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -399,31 +402,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4894F4A-9552-457D-9B25-E4ED232859CE}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
@@ -432,64 +441,67 @@
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>

</xml_diff>